<commit_message>
plots on seperate tabs
</commit_message>
<xml_diff>
--- a/testing/Joule Thief Measurments.xlsx
+++ b/testing/Joule Thief Measurments.xlsx
@@ -4,10 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14565" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14565" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Base Resistor Testing" sheetId="1" r:id="rId1"/>
+    <sheet name="LED on-off Voltage" sheetId="2" r:id="rId1"/>
+    <sheet name="Input Current" sheetId="3" r:id="rId2"/>
+    <sheet name="LED Light Output" sheetId="4" r:id="rId3"/>
+    <sheet name="Input Power" sheetId="5" r:id="rId4"/>
+    <sheet name="LED Light Outpu at Input Power" sheetId="6" r:id="rId5"/>
+    <sheet name="Base Resistor Testing" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="33">
   <si>
     <t>Current Sensor:</t>
   </si>
@@ -312,7 +317,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="22">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -405,9 +410,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -430,13 +432,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Voltage Level For Curcuit to Turn on/off at Base Resistor</a:t>
+              <a:t>LED on/off Voltage Vs Base Resistor Value</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Value</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -447,10 +444,10 @@
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Off</c:v>
+            <c:v>LED Turn On</c:v>
           </c:tx>
           <c:xVal>
             <c:numRef>
@@ -484,40 +481,40 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Base Resistor Testing'!$L$4:$L$10</c:f>
+              <c:f>'Base Resistor Testing'!$D$4:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.4002</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42780000000000001</c:v>
+                  <c:v>0.51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.46960000000000002</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53779999999999994</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.57630000000000003</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.58819999999999995</c:v>
+                  <c:v>0.59</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.60970000000000002</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>On</c:v>
+            <c:v>LED Turn Off</c:v>
           </c:tx>
           <c:xVal>
             <c:numRef>
@@ -551,40 +548,40 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Base Resistor Testing'!$M$4:$M$10</c:f>
+              <c:f>'Base Resistor Testing'!$C$4:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.52</c:v>
+                  <c:v>0.4002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.51</c:v>
+                  <c:v>0.42780000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.52</c:v>
+                  <c:v>0.46960000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.54</c:v>
+                  <c:v>0.53779999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.57630000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.59</c:v>
+                  <c:v>0.58819999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.6</c:v>
+                  <c:v>0.60970000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="119413760"/>
-        <c:axId val="119440128"/>
+        <c:axId val="169177472"/>
+        <c:axId val="169189376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119413760"/>
+        <c:axId val="169177472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -617,12 +614,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119440128"/>
+        <c:crossAx val="169189376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119440128"/>
+        <c:axId val="169189376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -639,7 +636,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Voltage</a:t>
+                  <a:t>Turn On/Off Voltage [volts]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -648,7 +645,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119413760"/>
+        <c:crossAx val="169177472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -659,11 +656,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1288,11 +1280,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="119468032"/>
-        <c:axId val="119469568"/>
+        <c:axId val="105540224"/>
+        <c:axId val="105558400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119468032"/>
+        <c:axId val="105540224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1317,12 +1309,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119469568"/>
+        <c:crossAx val="105558400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119469568"/>
+        <c:axId val="105558400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1348,7 +1340,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119468032"/>
+        <c:crossAx val="105540224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1359,11 +1351,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1988,11 +1975,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="119920128"/>
-        <c:axId val="119921664"/>
+        <c:axId val="79593856"/>
+        <c:axId val="79595776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119920128"/>
+        <c:axId val="79593856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2017,12 +2004,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119921664"/>
+        <c:crossAx val="79595776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119921664"/>
+        <c:axId val="79595776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2048,7 +2035,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119920128"/>
+        <c:crossAx val="79593856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2059,11 +2046,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -2688,11 +2670,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="109827968"/>
-        <c:axId val="109826432"/>
+        <c:axId val="156874240"/>
+        <c:axId val="157608192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109827968"/>
+        <c:axId val="156874240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2717,12 +2699,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109826432"/>
+        <c:crossAx val="157608192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109826432"/>
+        <c:axId val="157608192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2748,7 +2730,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109827968"/>
+        <c:crossAx val="156874240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2759,11 +2741,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -3388,11 +3365,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="155649920"/>
-        <c:axId val="155648000"/>
+        <c:axId val="79206272"/>
+        <c:axId val="79217024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="155649920"/>
+        <c:axId val="79206272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3421,12 +3398,12 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155648000"/>
+        <c:crossAx val="79217024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="155648000"/>
+        <c:axId val="79217024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3452,7 +3429,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155649920"/>
+        <c:crossAx val="79206272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3463,33 +3440,75 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>276225</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8656320" cy="6271260"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3502,24 +3521,21 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8656320" cy="6271260"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3527,29 +3543,26 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8656320" cy="6271260"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3557,29 +3570,26 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1038225</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8656320" cy="6271260"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3587,29 +3597,26 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1076325</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8656320" cy="6271260"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3617,41 +3624,20 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:M10" totalsRowShown="0" headerRowDxfId="22">
-  <autoFilter ref="B3:M10">
-    <filterColumn colId="4"/>
-    <filterColumn colId="8"/>
-    <filterColumn colId="9"/>
-  </autoFilter>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:D10" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="B3:D10"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="Base Resistor [Ω]"/>
-    <tableColumn id="9" name="Switching Frequency [kHz]"/>
-    <tableColumn id="2" name="Input Voltage [volts]"/>
-    <tableColumn id="3" name="Input Current [mA]"/>
-    <tableColumn id="12" name="Input Power [mW]" dataDxfId="21">
-      <calculatedColumnFormula>(D4 * (E4/1000))*1000</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" name="LED Current Sensor Voltage [volts]"/>
-    <tableColumn id="5" name="LED Current [mA]">
-      <calculatedColumnFormula>($P$5*G4)*1000</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" name="LED Light Level [volts]"/>
-    <tableColumn id="10" name="TEMT6000 Collector Current [uA]">
-      <calculatedColumnFormula>(I4/$P$9)*10^6</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="11" name="LED Light Level [lx]">
-      <calculatedColumnFormula>J4*2</calculatedColumnFormula>
-    </tableColumn>
     <tableColumn id="7" name="Turnoff Voltage [volts]"/>
     <tableColumn id="8" name="Turnon Voltage [volts]"/>
   </tableColumns>
@@ -3674,11 +3660,11 @@
     </tableColumn>
     <tableColumn id="5" name="LED Current Sensor Voltage [volts]"/>
     <tableColumn id="6" name="LED Current [mA]">
-      <calculatedColumnFormula>($P$5*G13)*1000</calculatedColumnFormula>
+      <calculatedColumnFormula>($N$5*G13)*1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="LED Light Level [volts]"/>
     <tableColumn id="8" name="TEMT6000 Collector Current [uA]">
-      <calculatedColumnFormula>(I13/$P$9)*10^6</calculatedColumnFormula>
+      <calculatedColumnFormula>(I13/$N$9)*10^6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="LED Light Level [lx]">
       <calculatedColumnFormula>J13*2</calculatedColumnFormula>
@@ -3703,11 +3689,11 @@
     </tableColumn>
     <tableColumn id="5" name="LED Current Sensor Voltage [volts]"/>
     <tableColumn id="6" name="LED Current [mA]">
-      <calculatedColumnFormula>($P$5*G25)*1000</calculatedColumnFormula>
+      <calculatedColumnFormula>($N$5*G25)*1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="LED Light Level [volts]"/>
     <tableColumn id="8" name="TEMT6000 Collector Current [uA]">
-      <calculatedColumnFormula>(I25/$P$9)*10^6</calculatedColumnFormula>
+      <calculatedColumnFormula>(I25/$N$9)*10^6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="LED Light Level [lx]">
       <calculatedColumnFormula>J25*2</calculatedColumnFormula>
@@ -3732,11 +3718,11 @@
     </tableColumn>
     <tableColumn id="5" name="LED Current Sensor Voltage [volts]"/>
     <tableColumn id="6" name="LED Current [mA]">
-      <calculatedColumnFormula>($P$5*G37)*1000</calculatedColumnFormula>
+      <calculatedColumnFormula>($N$5*G37)*1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="LED Light Level [volts]"/>
     <tableColumn id="8" name="TEMT6000 Collector Current [uA]">
-      <calculatedColumnFormula>(I37/$P$9)*10^6</calculatedColumnFormula>
+      <calculatedColumnFormula>(I37/$N$9)*10^6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="LED Light Level [lx]">
       <calculatedColumnFormula>J37*2</calculatedColumnFormula>
@@ -3761,11 +3747,11 @@
     </tableColumn>
     <tableColumn id="5" name="LED Current Sensor Voltage [volts]"/>
     <tableColumn id="6" name="LED Current [mA]">
-      <calculatedColumnFormula>($P$5*G50)*1000</calculatedColumnFormula>
+      <calculatedColumnFormula>($N$5*G50)*1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="LED Light Level [volts]"/>
     <tableColumn id="8" name="TEMT6000 Collector Current [uA]">
-      <calculatedColumnFormula>(I50/$P$9)*10^6</calculatedColumnFormula>
+      <calculatedColumnFormula>(I50/$N$9)*10^6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="LED Light Level [lx]">
       <calculatedColumnFormula>J50*2</calculatedColumnFormula>
@@ -3790,11 +3776,11 @@
     </tableColumn>
     <tableColumn id="5" name="LED Current Sensor Voltage [volts]"/>
     <tableColumn id="6" name="LED Current [mA]">
-      <calculatedColumnFormula>($P$5*G62)*1000</calculatedColumnFormula>
+      <calculatedColumnFormula>($N$5*G62)*1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="LED Light Level [volts]"/>
     <tableColumn id="8" name="TEMT6000 Collector Current [uA]">
-      <calculatedColumnFormula>(I62/$P$9)*10^6</calculatedColumnFormula>
+      <calculatedColumnFormula>(I62/$N$9)*10^6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="LED Light Level [lx]">
       <calculatedColumnFormula>J62*2</calculatedColumnFormula>
@@ -3819,11 +3805,11 @@
     </tableColumn>
     <tableColumn id="5" name="LED Current Sensor Voltage [volts]"/>
     <tableColumn id="6" name="LED Current [mA]">
-      <calculatedColumnFormula>($P$5*G74)*1000</calculatedColumnFormula>
+      <calculatedColumnFormula>($N$5*G74)*1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="LED Light Level [volts]"/>
     <tableColumn id="8" name="TEMT6000 Collector Current [uA]">
-      <calculatedColumnFormula>(I74/$P$9)*10^6</calculatedColumnFormula>
+      <calculatedColumnFormula>(I74/$N$9)*10^6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="LED Light Level [lx]">
       <calculatedColumnFormula>J74*2</calculatedColumnFormula>
@@ -3848,11 +3834,11 @@
     </tableColumn>
     <tableColumn id="5" name="LED Current Sensor Voltage [volts]"/>
     <tableColumn id="6" name="LED Current [mA]">
-      <calculatedColumnFormula>($P$5*G86)*1000</calculatedColumnFormula>
+      <calculatedColumnFormula>($N$5*G86)*1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="LED Light Level [volts]"/>
     <tableColumn id="8" name="TEMT6000 Collector Current [uA]">
-      <calculatedColumnFormula>(I86/$P$9)*10^6</calculatedColumnFormula>
+      <calculatedColumnFormula>(I86/$N$9)*10^6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="LED Light Level [lx]">
       <calculatedColumnFormula>J86*2</calculatedColumnFormula>
@@ -4184,40 +4170,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:Q96"/>
+  <dimension ref="A2:O96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A10"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
     <col min="4" max="4" width="12.875" customWidth="1"/>
     <col min="5" max="5" width="12.75" customWidth="1"/>
     <col min="6" max="6" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="11.375" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="13.75" customWidth="1"/>
     <col min="9" max="9" width="18.125" customWidth="1"/>
-    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="10" max="10" width="18.625" customWidth="1"/>
     <col min="11" max="11" width="14.375" customWidth="1"/>
     <col min="12" max="12" width="14.25" customWidth="1"/>
-    <col min="14" max="14" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.25" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:15">
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
       <c r="N2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="30" customHeight="1">
+    <row r="3" spans="1:15" ht="30" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>31</v>
       </c>
@@ -4225,386 +4212,142 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="M3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>200</v>
+      </c>
       <c r="O3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3">
-        <v>200</v>
-      </c>
-      <c r="Q3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:15">
       <c r="A4" s="6"/>
       <c r="B4">
         <v>1000</v>
       </c>
       <c r="C4">
-        <v>102.3</v>
+        <v>0.4002</v>
       </c>
       <c r="D4">
-        <v>0.80259999999999998</v>
-      </c>
-      <c r="E4">
-        <v>36.83</v>
-      </c>
-      <c r="F4" s="4">
-        <f t="shared" ref="F4:F10" si="0">(D4 * (E4/1000))*1000</f>
-        <v>29.559758000000002</v>
-      </c>
-      <c r="G4">
-        <v>0.1038</v>
-      </c>
-      <c r="H4">
-        <f t="shared" ref="H4:H10" si="1">($P$5*G4)*1000</f>
-        <v>5.19</v>
-      </c>
-      <c r="I4">
-        <v>2.859</v>
-      </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J10" si="2">(I4/$P$9)*10^6</f>
-        <v>285.90000000000003</v>
-      </c>
-      <c r="K4">
-        <f t="shared" ref="K4:K10" si="3">J4*2</f>
-        <v>571.80000000000007</v>
-      </c>
-      <c r="L4">
-        <v>0.4002</v>
-      </c>
-      <c r="M4">
         <v>0.52</v>
       </c>
+      <c r="M4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>0.1</v>
+      </c>
       <c r="O4" t="s">
-        <v>4</v>
-      </c>
-      <c r="P4">
-        <v>0.1</v>
-      </c>
-      <c r="Q4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:15">
       <c r="A5" s="6"/>
       <c r="B5">
         <v>1500</v>
       </c>
       <c r="C5">
-        <v>109.2</v>
+        <v>0.42780000000000001</v>
       </c>
       <c r="D5">
-        <v>0.80510000000000004</v>
-      </c>
-      <c r="E5">
-        <v>34.15</v>
-      </c>
-      <c r="F5" s="4">
-        <f t="shared" si="0"/>
-        <v>27.494165000000002</v>
-      </c>
-      <c r="G5">
-        <v>9.7299999999999998E-2</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>4.8650000000000002</v>
-      </c>
-      <c r="I5">
-        <v>2.7320000000000002</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="2"/>
-        <v>273.20000000000005</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="3"/>
-        <v>546.40000000000009</v>
-      </c>
-      <c r="L5">
-        <v>0.42780000000000001</v>
-      </c>
-      <c r="M5">
         <v>0.51</v>
       </c>
-      <c r="O5" t="s">
+      <c r="M5" t="s">
         <v>6</v>
       </c>
-      <c r="P5">
+      <c r="N5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:15">
       <c r="A6" s="6"/>
       <c r="B6">
         <v>2200</v>
       </c>
       <c r="C6">
-        <v>119.4</v>
+        <v>0.46960000000000002</v>
       </c>
       <c r="D6">
-        <v>0.80120000000000002</v>
-      </c>
-      <c r="E6">
-        <v>30.69</v>
-      </c>
-      <c r="F6" s="4">
-        <f t="shared" si="0"/>
-        <v>24.588828000000003</v>
-      </c>
-      <c r="G6">
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>4.3749999999999991</v>
-      </c>
-      <c r="I6">
-        <v>2.5249999999999999</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
-        <v>252.5</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="3"/>
-        <v>505</v>
-      </c>
-      <c r="L6">
-        <v>0.46960000000000002</v>
-      </c>
-      <c r="M6">
         <v>0.52</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:15">
       <c r="A7" s="6"/>
       <c r="B7">
         <v>3300</v>
       </c>
       <c r="C7">
-        <v>133</v>
+        <v>0.53779999999999994</v>
       </c>
       <c r="D7">
-        <v>0.80279999999999996</v>
-      </c>
-      <c r="E7">
-        <v>27.06</v>
-      </c>
-      <c r="F7" s="4">
-        <f t="shared" si="0"/>
-        <v>21.723767999999996</v>
-      </c>
-      <c r="G7">
-        <v>7.7200000000000005E-2</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>3.8600000000000008</v>
-      </c>
-      <c r="I7">
-        <v>2.2970000000000002</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
-        <v>229.70000000000002</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="3"/>
-        <v>459.40000000000003</v>
-      </c>
-      <c r="L7">
-        <v>0.53779999999999994</v>
-      </c>
-      <c r="M7">
         <v>0.54</v>
       </c>
-      <c r="O7" t="s">
+      <c r="M7" t="s">
         <v>14</v>
       </c>
-      <c r="P7" t="s">
+      <c r="N7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:15">
       <c r="A8" s="6"/>
       <c r="B8">
         <v>4700</v>
       </c>
       <c r="C8">
-        <v>142.19999999999999</v>
+        <v>0.57630000000000003</v>
       </c>
       <c r="D8">
-        <v>0.80389999999999995</v>
-      </c>
-      <c r="E8">
-        <v>20.558</v>
-      </c>
-      <c r="F8" s="4">
-        <f t="shared" si="0"/>
-        <v>16.526576200000001</v>
-      </c>
-      <c r="G8">
-        <v>5.6300000000000003E-2</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
-        <v>2.8150000000000004</v>
-      </c>
-      <c r="I8">
-        <v>1.7549999999999999</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="2"/>
-        <v>175.49999999999997</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="3"/>
-        <v>350.99999999999994</v>
-      </c>
-      <c r="L8">
-        <v>0.57630000000000003</v>
-      </c>
-      <c r="M8">
         <v>0.57999999999999996</v>
       </c>
-      <c r="O8" t="s">
+      <c r="M8" t="s">
         <v>16</v>
       </c>
-      <c r="P8" t="s">
+      <c r="N8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:15">
       <c r="A9" s="6"/>
       <c r="B9">
         <v>5600</v>
       </c>
       <c r="C9">
-        <v>148.9</v>
+        <v>0.58819999999999995</v>
       </c>
       <c r="D9">
-        <v>0.80500000000000005</v>
-      </c>
-      <c r="E9">
-        <v>17.809999999999999</v>
-      </c>
-      <c r="F9" s="4">
-        <f t="shared" si="0"/>
-        <v>14.33705</v>
-      </c>
-      <c r="G9">
-        <v>4.7899999999999998E-2</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>2.395</v>
-      </c>
-      <c r="I9">
-        <v>1.5209999999999999</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="2"/>
-        <v>152.1</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="3"/>
-        <v>304.2</v>
-      </c>
-      <c r="L9">
-        <v>0.58819999999999995</v>
-      </c>
-      <c r="M9">
         <v>0.59</v>
       </c>
+      <c r="M9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9">
+        <v>10000</v>
+      </c>
       <c r="O9" t="s">
-        <v>30</v>
-      </c>
-      <c r="P9">
-        <v>10000</v>
-      </c>
-      <c r="Q9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:15">
       <c r="A10" s="6"/>
       <c r="B10">
         <v>6800</v>
       </c>
       <c r="C10">
-        <v>161</v>
+        <v>0.60970000000000002</v>
       </c>
       <c r="D10">
-        <v>0.80559999999999998</v>
-      </c>
-      <c r="E10">
-        <v>15.164</v>
-      </c>
-      <c r="F10" s="4">
-        <f t="shared" si="0"/>
-        <v>12.216118399999999</v>
-      </c>
-      <c r="G10">
-        <v>3.9300000000000002E-2</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
-        <v>1.9650000000000001</v>
-      </c>
-      <c r="I10">
-        <v>1.2749999999999999</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="2"/>
-        <v>127.49999999999999</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="3"/>
-        <v>254.99999999999997</v>
-      </c>
-      <c r="L10">
-        <v>0.60970000000000002</v>
-      </c>
-      <c r="M10">
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:15">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -4613,7 +4356,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="30" customHeight="1">
+    <row r="12" spans="1:15" ht="30" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -4648,7 +4391,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:15">
       <c r="A13" s="5"/>
       <c r="B13">
         <v>1000</v>
@@ -4663,29 +4406,29 @@
         <v>129.62</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" ref="F13:F22" si="4">(D13 * (E13/1000))*1000</f>
+        <f t="shared" ref="F13:F22" si="0">(D13 * (E13/1000))*1000</f>
         <v>195.11698600000003</v>
       </c>
       <c r="G13">
         <v>0.57999999999999996</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="H13:H22" si="5">($P$5*G13)*1000</f>
+        <f>($N$5*G13)*1000</f>
         <v>28.999999999999996</v>
       </c>
       <c r="I13">
         <v>3.181</v>
       </c>
       <c r="J13">
-        <f t="shared" ref="J13:J22" si="6">(I13/$P$9)*10^6</f>
+        <f>(I13/$N$9)*10^6</f>
         <v>318.09999999999997</v>
       </c>
       <c r="K13">
-        <f t="shared" ref="K13:K22" si="7">J13*2</f>
+        <f t="shared" ref="K13:K22" si="1">J13*2</f>
         <v>636.19999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:15">
       <c r="A14" s="5"/>
       <c r="B14">
         <v>1000</v>
@@ -4700,29 +4443,29 @@
         <v>112.94</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>158.307998</v>
       </c>
       <c r="G14">
         <v>0.47449999999999998</v>
       </c>
       <c r="H14">
-        <f t="shared" si="5"/>
+        <f>($N$5*G14)*1000</f>
         <v>23.724999999999998</v>
       </c>
       <c r="I14">
         <v>3.1749999999999998</v>
       </c>
       <c r="J14">
-        <f t="shared" si="6"/>
+        <f>(I14/$N$9)*10^6</f>
         <v>317.49999999999994</v>
       </c>
       <c r="K14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>634.99999999999989</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:15">
       <c r="A15" s="5"/>
       <c r="B15">
         <v>1000</v>
@@ -4737,29 +4480,29 @@
         <v>99.9</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>130.46940000000001</v>
       </c>
       <c r="G15">
         <v>0.39400000000000002</v>
       </c>
       <c r="H15">
-        <f t="shared" si="5"/>
+        <f>($N$5*G15)*1000</f>
         <v>19.700000000000003</v>
       </c>
       <c r="I15">
         <v>3.169</v>
       </c>
       <c r="J15">
-        <f t="shared" si="6"/>
+        <f>(I15/$N$9)*10^6</f>
         <v>316.89999999999998</v>
       </c>
       <c r="K15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>633.79999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:15">
       <c r="A16" s="5"/>
       <c r="B16">
         <v>1000</v>
@@ -4774,25 +4517,25 @@
         <v>88.09</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>105.875371</v>
       </c>
       <c r="G16">
         <v>0.32</v>
       </c>
       <c r="H16">
-        <f t="shared" si="5"/>
+        <f>($N$5*G16)*1000</f>
         <v>16</v>
       </c>
       <c r="I16">
         <v>3.1659999999999999</v>
       </c>
       <c r="J16">
-        <f t="shared" si="6"/>
+        <f>(I16/$N$9)*10^6</f>
         <v>316.60000000000002</v>
       </c>
       <c r="K16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>633.20000000000005</v>
       </c>
     </row>
@@ -4811,25 +4554,25 @@
         <v>77.02</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>84.891443999999993</v>
       </c>
       <c r="G17">
         <v>0.26200000000000001</v>
       </c>
       <c r="H17">
-        <f t="shared" si="5"/>
+        <f>($N$5*G17)*1000</f>
         <v>13.100000000000001</v>
       </c>
       <c r="I17">
         <v>3.1640000000000001</v>
       </c>
       <c r="J17">
-        <f t="shared" si="6"/>
+        <f>(I17/$N$9)*10^6</f>
         <v>316.39999999999998</v>
       </c>
       <c r="K17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>632.79999999999995</v>
       </c>
     </row>
@@ -4848,25 +4591,25 @@
         <v>62.96</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>63.129991999999994</v>
       </c>
       <c r="G18">
         <v>0.20050000000000001</v>
       </c>
       <c r="H18">
-        <f t="shared" si="5"/>
+        <f>($N$5*G18)*1000</f>
         <v>10.025</v>
       </c>
       <c r="I18">
         <v>3.16</v>
       </c>
       <c r="J18">
-        <f t="shared" si="6"/>
+        <f>(I18/$N$9)*10^6</f>
         <v>316.00000000000006</v>
       </c>
       <c r="K18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>632.00000000000011</v>
       </c>
     </row>
@@ -4885,25 +4628,25 @@
         <v>46.12</v>
       </c>
       <c r="F19" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>41.627911999999995</v>
       </c>
       <c r="G19">
         <v>0.13900000000000001</v>
       </c>
       <c r="H19">
-        <f t="shared" si="5"/>
+        <f>($N$5*G19)*1000</f>
         <v>6.9500000000000011</v>
       </c>
       <c r="I19">
         <v>3.137</v>
       </c>
       <c r="J19">
-        <f t="shared" si="6"/>
+        <f>(I19/$N$9)*10^6</f>
         <v>313.7</v>
       </c>
       <c r="K19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>627.4</v>
       </c>
     </row>
@@ -4922,25 +4665,25 @@
         <v>36.36</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>29.091635999999998</v>
       </c>
       <c r="G20">
         <v>0.10299999999999999</v>
       </c>
       <c r="H20">
-        <f t="shared" si="5"/>
+        <f>($N$5*G20)*1000</f>
         <v>5.15</v>
       </c>
       <c r="I20">
         <v>2.8410000000000002</v>
       </c>
       <c r="J20">
-        <f t="shared" si="6"/>
+        <f>(I20/$N$9)*10^6</f>
         <v>284.10000000000002</v>
       </c>
       <c r="K20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>568.20000000000005</v>
       </c>
     </row>
@@ -4959,25 +4702,25 @@
         <v>28.7</v>
       </c>
       <c r="F21" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>20.233499999999999</v>
       </c>
       <c r="G21">
         <v>7.4300000000000005E-2</v>
       </c>
       <c r="H21">
-        <f t="shared" si="5"/>
+        <f>($N$5*G21)*1000</f>
         <v>3.7150000000000003</v>
       </c>
       <c r="I21">
         <v>2.181</v>
       </c>
       <c r="J21">
-        <f t="shared" si="6"/>
+        <f>(I21/$N$9)*10^6</f>
         <v>218.10000000000002</v>
       </c>
       <c r="K21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>436.20000000000005</v>
       </c>
     </row>
@@ -4996,25 +4739,25 @@
         <v>20.472999999999999</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>12.334982499999999</v>
       </c>
       <c r="G22">
         <v>4.7E-2</v>
       </c>
       <c r="H22">
-        <f t="shared" si="5"/>
+        <f>($N$5*G22)*1000</f>
         <v>2.35</v>
       </c>
       <c r="I22">
         <v>1.4570000000000001</v>
       </c>
       <c r="J22">
-        <f t="shared" si="6"/>
+        <f>(I22/$N$9)*10^6</f>
         <v>145.70000000000002</v>
       </c>
       <c r="K22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>291.40000000000003</v>
       </c>
     </row>
@@ -5068,25 +4811,25 @@
         <v>111.5</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" ref="F25:F34" si="8">(D25 * (E25/1000))*1000</f>
+        <f t="shared" ref="F25:F34" si="2">(D25 * (E25/1000))*1000</f>
         <v>168.14200000000002</v>
       </c>
       <c r="G25">
         <v>0.54</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25:H34" si="9">($P$5*G25)*1000</f>
+        <f>($N$5*G25)*1000</f>
         <v>27.000000000000004</v>
       </c>
       <c r="I25">
         <v>3.1840000000000002</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25:J34" si="10">(I25/$P$9)*10^6</f>
+        <f>(I25/$N$9)*10^6</f>
         <v>318.40000000000003</v>
       </c>
       <c r="K25">
-        <f t="shared" ref="K25:K34" si="11">J25*2</f>
+        <f t="shared" ref="K25:K34" si="3">J25*2</f>
         <v>636.80000000000007</v>
       </c>
     </row>
@@ -5105,25 +4848,25 @@
         <v>97.8</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>137.5068</v>
       </c>
       <c r="G26">
         <v>0.44400000000000001</v>
       </c>
       <c r="H26">
-        <f t="shared" si="9"/>
+        <f>($N$5*G26)*1000</f>
         <v>22.2</v>
       </c>
       <c r="I26">
         <v>3.1789999999999998</v>
       </c>
       <c r="J26">
-        <f t="shared" si="10"/>
+        <f>(I26/$N$9)*10^6</f>
         <v>317.89999999999998</v>
       </c>
       <c r="K26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>635.79999999999995</v>
       </c>
     </row>
@@ -5142,25 +4885,25 @@
         <v>86.6</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>112.66659999999999</v>
       </c>
       <c r="G27">
         <v>0.36399999999999999</v>
       </c>
       <c r="H27">
-        <f t="shared" si="9"/>
+        <f>($N$5*G27)*1000</f>
         <v>18.2</v>
       </c>
       <c r="I27">
         <v>3.1749999999999998</v>
       </c>
       <c r="J27">
-        <f t="shared" si="10"/>
+        <f>(I27/$N$9)*10^6</f>
         <v>317.49999999999994</v>
       </c>
       <c r="K27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>634.99999999999989</v>
       </c>
     </row>
@@ -5179,25 +4922,25 @@
         <v>77.5</v>
       </c>
       <c r="F28" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>93.542500000000004</v>
       </c>
       <c r="G28">
         <v>0.30199999999999999</v>
       </c>
       <c r="H28">
-        <f t="shared" si="9"/>
+        <f>($N$5*G28)*1000</f>
         <v>15.100000000000001</v>
       </c>
       <c r="I28">
         <v>3.1720000000000002</v>
       </c>
       <c r="J28">
-        <f t="shared" si="10"/>
+        <f>(I28/$N$9)*10^6</f>
         <v>317.2</v>
       </c>
       <c r="K28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>634.4</v>
       </c>
     </row>
@@ -5216,25 +4959,25 @@
         <v>66.7</v>
       </c>
       <c r="F29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>73.836900000000014</v>
       </c>
       <c r="G29">
         <v>0.24099999999999999</v>
       </c>
       <c r="H29">
-        <f t="shared" si="9"/>
+        <f>($N$5*G29)*1000</f>
         <v>12.05</v>
       </c>
       <c r="I29">
         <v>3.169</v>
       </c>
       <c r="J29">
-        <f t="shared" si="10"/>
+        <f>(I29/$N$9)*10^6</f>
         <v>316.89999999999998</v>
       </c>
       <c r="K29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>633.79999999999995</v>
       </c>
     </row>
@@ -5253,25 +4996,25 @@
         <v>51.2</v>
       </c>
       <c r="F30" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>51.3536</v>
       </c>
       <c r="G30">
         <v>0.17100000000000001</v>
       </c>
       <c r="H30">
-        <f t="shared" si="9"/>
+        <f>($N$5*G30)*1000</f>
         <v>8.5500000000000007</v>
       </c>
       <c r="I30">
         <v>3.1560000000000001</v>
       </c>
       <c r="J30">
-        <f t="shared" si="10"/>
+        <f>(I30/$N$9)*10^6</f>
         <v>315.60000000000002</v>
       </c>
       <c r="K30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>631.20000000000005</v>
       </c>
     </row>
@@ -5290,25 +5033,25 @@
         <v>41.1</v>
       </c>
       <c r="F31" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>37.031100000000002</v>
       </c>
       <c r="G31">
         <v>0.128</v>
       </c>
       <c r="H31">
-        <f t="shared" si="9"/>
+        <f>($N$5*G31)*1000</f>
         <v>6.4</v>
       </c>
       <c r="I31">
         <v>3.1230000000000002</v>
       </c>
       <c r="J31">
-        <f t="shared" si="10"/>
+        <f>(I31/$N$9)*10^6</f>
         <v>312.3</v>
       </c>
       <c r="K31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>624.6</v>
       </c>
     </row>
@@ -5327,25 +5070,25 @@
         <v>33.700000000000003</v>
       </c>
       <c r="F32" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>27.027400000000004</v>
       </c>
       <c r="G32">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="H32">
-        <f t="shared" si="9"/>
+        <f>($N$5*G32)*1000</f>
         <v>4.8000000000000007</v>
       </c>
       <c r="I32">
         <v>2.7050000000000001</v>
       </c>
       <c r="J32">
-        <f t="shared" si="10"/>
+        <f>(I32/$N$9)*10^6</f>
         <v>270.5</v>
       </c>
       <c r="K32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>541</v>
       </c>
     </row>
@@ -5364,25 +5107,25 @@
         <v>26.6</v>
       </c>
       <c r="F33" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>18.646599999999999</v>
       </c>
       <c r="G33">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="H33">
-        <f t="shared" si="9"/>
+        <f>($N$5*G33)*1000</f>
         <v>3.4000000000000004</v>
       </c>
       <c r="I33">
         <v>2.0299999999999998</v>
       </c>
       <c r="J33">
-        <f t="shared" si="10"/>
+        <f>(I33/$N$9)*10^6</f>
         <v>202.99999999999997</v>
       </c>
       <c r="K33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>405.99999999999994</v>
       </c>
     </row>
@@ -5401,25 +5144,25 @@
         <v>19.2</v>
       </c>
       <c r="F34" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>11.577599999999999</v>
       </c>
       <c r="G34">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="H34">
-        <f t="shared" si="9"/>
+        <f>($N$5*G34)*1000</f>
         <v>2.15</v>
       </c>
       <c r="I34">
         <v>1.349</v>
       </c>
       <c r="J34">
-        <f t="shared" si="10"/>
+        <f>(I34/$N$9)*10^6</f>
         <v>134.9</v>
       </c>
       <c r="K34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>269.8</v>
       </c>
     </row>
@@ -5481,25 +5224,25 @@
         <v>93.6</v>
       </c>
       <c r="F37" s="4">
-        <f t="shared" ref="F37:F46" si="12">(D37 * (E37/1000))*1000</f>
+        <f t="shared" ref="F37:F46" si="4">(D37 * (E37/1000))*1000</f>
         <v>140.5872</v>
       </c>
       <c r="G37">
         <v>0.48399999999999999</v>
       </c>
       <c r="H37">
-        <f t="shared" ref="H37:H46" si="13">($P$5*G37)*1000</f>
+        <f>($N$5*G37)*1000</f>
         <v>24.2</v>
       </c>
       <c r="I37">
         <v>3.1869999999999998</v>
       </c>
       <c r="J37">
-        <f t="shared" ref="J37:J46" si="14">(I37/$P$9)*10^6</f>
+        <f>(I37/$N$9)*10^6</f>
         <v>318.7</v>
       </c>
       <c r="K37">
-        <f t="shared" ref="K37:K46" si="15">J37*2</f>
+        <f t="shared" ref="K37:K46" si="5">J37*2</f>
         <v>637.4</v>
       </c>
     </row>
@@ -5518,25 +5261,25 @@
         <v>84.2</v>
       </c>
       <c r="F38" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>118.55359999999999</v>
       </c>
       <c r="G38">
         <v>0.40699999999999997</v>
       </c>
       <c r="H38">
-        <f t="shared" si="13"/>
+        <f>($N$5*G38)*1000</f>
         <v>20.350000000000001</v>
       </c>
       <c r="I38">
         <v>3.1840000000000002</v>
       </c>
       <c r="J38">
-        <f t="shared" si="14"/>
+        <f>(I38/$N$9)*10^6</f>
         <v>318.40000000000003</v>
       </c>
       <c r="K38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>636.80000000000007</v>
       </c>
     </row>
@@ -5555,25 +5298,25 @@
         <v>75.099999999999994</v>
       </c>
       <c r="F39" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>97.930400000000006</v>
       </c>
       <c r="G39">
         <v>0.33500000000000002</v>
       </c>
       <c r="H39">
-        <f t="shared" si="13"/>
+        <f>($N$5*G39)*1000</f>
         <v>16.75</v>
       </c>
       <c r="I39">
         <v>3.18</v>
       </c>
       <c r="J39">
-        <f t="shared" si="14"/>
+        <f>(I39/$N$9)*10^6</f>
         <v>318.00000000000006</v>
       </c>
       <c r="K39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>636.00000000000011</v>
       </c>
     </row>
@@ -5592,25 +5335,25 @@
         <v>66.099999999999994</v>
       </c>
       <c r="F40" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>79.848799999999983</v>
       </c>
       <c r="G40">
         <v>0.27200000000000002</v>
       </c>
       <c r="H40">
-        <f t="shared" si="13"/>
+        <f>($N$5*G40)*1000</f>
         <v>13.600000000000001</v>
       </c>
       <c r="I40">
         <v>3.1760000000000002</v>
       </c>
       <c r="J40">
-        <f t="shared" si="14"/>
+        <f>(I40/$N$9)*10^6</f>
         <v>317.60000000000002</v>
       </c>
       <c r="K40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>635.20000000000005</v>
       </c>
     </row>
@@ -5629,25 +5372,25 @@
         <v>53.4</v>
       </c>
       <c r="F41" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>59.006999999999998</v>
       </c>
       <c r="G41">
         <v>0.20100000000000001</v>
       </c>
       <c r="H41">
-        <f t="shared" si="13"/>
+        <f>($N$5*G41)*1000</f>
         <v>10.050000000000002</v>
       </c>
       <c r="I41">
         <v>3.1669999999999998</v>
       </c>
       <c r="J41">
-        <f t="shared" si="14"/>
+        <f>(I41/$N$9)*10^6</f>
         <v>316.7</v>
       </c>
       <c r="K41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>633.4</v>
       </c>
     </row>
@@ -5666,25 +5409,25 @@
         <v>43.3</v>
       </c>
       <c r="F42" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>43.343299999999992</v>
       </c>
       <c r="G42">
         <v>0.15</v>
       </c>
       <c r="H42">
-        <f t="shared" si="13"/>
+        <f>($N$5*G42)*1000</f>
         <v>7.5</v>
       </c>
       <c r="I42">
         <v>3.149</v>
       </c>
       <c r="J42">
-        <f t="shared" si="14"/>
+        <f>(I42/$N$9)*10^6</f>
         <v>314.90000000000003</v>
       </c>
       <c r="K42">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>629.80000000000007</v>
       </c>
     </row>
@@ -5703,25 +5446,25 @@
         <v>37</v>
       </c>
       <c r="F43" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>33.448</v>
       </c>
       <c r="G43">
         <v>0.11799999999999999</v>
       </c>
       <c r="H43">
-        <f t="shared" si="13"/>
+        <f>($N$5*G43)*1000</f>
         <v>5.8999999999999995</v>
       </c>
       <c r="I43">
         <v>3.0950000000000002</v>
       </c>
       <c r="J43">
-        <f t="shared" si="14"/>
+        <f>(I43/$N$9)*10^6</f>
         <v>309.50000000000006</v>
       </c>
       <c r="K43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>619.00000000000011</v>
       </c>
     </row>
@@ -5740,25 +5483,25 @@
         <v>30.8</v>
       </c>
       <c r="F44" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>24.8248</v>
       </c>
       <c r="G44">
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="H44">
-        <f t="shared" si="13"/>
+        <f>($N$5*G44)*1000</f>
         <v>4.45</v>
       </c>
       <c r="I44">
         <v>2.5550000000000002</v>
       </c>
       <c r="J44">
-        <f t="shared" si="14"/>
+        <f>(I44/$N$9)*10^6</f>
         <v>255.50000000000003</v>
       </c>
       <c r="K44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>511.00000000000006</v>
       </c>
     </row>
@@ -5777,25 +5520,25 @@
         <v>24.9</v>
       </c>
       <c r="F45" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>17.454899999999999</v>
       </c>
       <c r="G45">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="H45">
-        <f t="shared" si="13"/>
+        <f>($N$5*G45)*1000</f>
         <v>3.0500000000000003</v>
       </c>
       <c r="I45">
         <v>1.8620000000000001</v>
       </c>
       <c r="J45">
-        <f t="shared" si="14"/>
+        <f>(I45/$N$9)*10^6</f>
         <v>186.2</v>
       </c>
       <c r="K45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>372.4</v>
       </c>
     </row>
@@ -5814,25 +5557,25 @@
         <v>17</v>
       </c>
       <c r="F46" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>10.200000000000001</v>
       </c>
       <c r="G46">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="H46">
-        <f t="shared" si="13"/>
+        <f>($N$5*G46)*1000</f>
         <v>1.85</v>
       </c>
       <c r="I46">
         <v>1.1679999999999999</v>
       </c>
       <c r="J46">
-        <f t="shared" si="14"/>
+        <f>(I46/$N$9)*10^6</f>
         <v>116.8</v>
       </c>
       <c r="K46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>233.6</v>
       </c>
     </row>
@@ -5894,25 +5637,25 @@
         <v>80.3</v>
       </c>
       <c r="F50" s="4">
-        <f t="shared" ref="F50:F59" si="16">(D50 * (E50/1000))*1000</f>
+        <f t="shared" ref="F50:F59" si="6">(D50 * (E50/1000))*1000</f>
         <v>121.57419999999999</v>
       </c>
       <c r="G50">
         <v>0.443</v>
       </c>
       <c r="H50">
-        <f t="shared" ref="H50:H59" si="17">($P$5*G50)*1000</f>
+        <f>($N$5*G50)*1000</f>
         <v>22.150000000000002</v>
       </c>
       <c r="I50">
         <v>3.1920000000000002</v>
       </c>
       <c r="J50">
-        <f t="shared" ref="J50:J59" si="18">(I50/$P$9)*10^6</f>
+        <f>(I50/$N$9)*10^6</f>
         <v>319.2</v>
       </c>
       <c r="K50">
-        <f t="shared" ref="K50:K59" si="19">J50*2</f>
+        <f t="shared" ref="K50:K59" si="7">J50*2</f>
         <v>638.4</v>
       </c>
     </row>
@@ -5931,25 +5674,25 @@
         <v>71.3</v>
       </c>
       <c r="F51" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v>99.962599999999995</v>
       </c>
       <c r="G51">
         <v>0.36199999999999999</v>
       </c>
       <c r="H51">
-        <f t="shared" si="17"/>
+        <f>($N$5*G51)*1000</f>
         <v>18.100000000000001</v>
       </c>
       <c r="I51">
         <v>3.1880000000000002</v>
       </c>
       <c r="J51">
-        <f t="shared" si="18"/>
+        <f>(I51/$N$9)*10^6</f>
         <v>318.8</v>
       </c>
       <c r="K51">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>637.6</v>
       </c>
     </row>
@@ -5968,25 +5711,25 @@
         <v>62.7</v>
       </c>
       <c r="F52" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v>81.948900000000009</v>
       </c>
       <c r="G52">
         <v>0.29199999999999998</v>
       </c>
       <c r="H52">
-        <f t="shared" si="17"/>
+        <f>($N$5*G52)*1000</f>
         <v>14.6</v>
       </c>
       <c r="I52">
         <v>3.1829999999999998</v>
       </c>
       <c r="J52">
-        <f t="shared" si="18"/>
+        <f>(I52/$N$9)*10^6</f>
         <v>318.3</v>
       </c>
       <c r="K52">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>636.6</v>
       </c>
     </row>
@@ -6005,25 +5748,25 @@
         <v>52</v>
       </c>
       <c r="F53" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v>62.764000000000003</v>
       </c>
       <c r="G53">
         <v>0.224</v>
       </c>
       <c r="H53">
-        <f t="shared" si="17"/>
+        <f>($N$5*G53)*1000</f>
         <v>11.200000000000001</v>
       </c>
       <c r="I53">
         <v>3.1749999999999998</v>
       </c>
       <c r="J53">
-        <f t="shared" si="18"/>
+        <f>(I53/$N$9)*10^6</f>
         <v>317.49999999999994</v>
       </c>
       <c r="K53">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>634.99999999999989</v>
       </c>
     </row>
@@ -6042,25 +5785,25 @@
         <v>42.7</v>
       </c>
       <c r="F54" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v>47.226200000000006</v>
       </c>
       <c r="G54">
         <v>0.16800000000000001</v>
       </c>
       <c r="H54">
-        <f t="shared" si="17"/>
+        <f>($N$5*G54)*1000</f>
         <v>8.4</v>
       </c>
       <c r="I54">
         <v>3.16</v>
       </c>
       <c r="J54">
-        <f t="shared" si="18"/>
+        <f>(I54/$N$9)*10^6</f>
         <v>316.00000000000006</v>
       </c>
       <c r="K54">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>632.00000000000011</v>
       </c>
     </row>
@@ -6079,25 +5822,25 @@
         <v>37.5</v>
       </c>
       <c r="F55" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v>37.65</v>
       </c>
       <c r="G55">
         <v>0.13400000000000001</v>
       </c>
       <c r="H55">
-        <f t="shared" si="17"/>
+        <f>($N$5*G55)*1000</f>
         <v>6.7000000000000011</v>
       </c>
       <c r="I55">
         <v>3.137</v>
       </c>
       <c r="J55">
-        <f t="shared" si="18"/>
+        <f>(I55/$N$9)*10^6</f>
         <v>313.7</v>
       </c>
       <c r="K55">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>627.4</v>
       </c>
     </row>
@@ -6116,25 +5859,25 @@
         <v>32.5</v>
       </c>
       <c r="F56" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v>29.51</v>
       </c>
       <c r="G56">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="H56">
-        <f t="shared" si="17"/>
+        <f>($N$5*G56)*1000</f>
         <v>4.8000000000000007</v>
       </c>
       <c r="I56">
         <v>2.7469999999999999</v>
       </c>
       <c r="J56">
-        <f t="shared" si="18"/>
+        <f>(I56/$N$9)*10^6</f>
         <v>274.7</v>
       </c>
       <c r="K56">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>549.4</v>
       </c>
     </row>
@@ -6153,25 +5896,25 @@
         <v>26.4</v>
       </c>
       <c r="F57" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v>21.2256</v>
       </c>
       <c r="G57">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="H57">
-        <f t="shared" si="17"/>
+        <f>($N$5*G57)*1000</f>
         <v>3.8</v>
       </c>
       <c r="I57">
         <v>2.2570000000000001</v>
       </c>
       <c r="J57">
-        <f t="shared" si="18"/>
+        <f>(I57/$N$9)*10^6</f>
         <v>225.70000000000002</v>
       </c>
       <c r="K57">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>451.40000000000003</v>
       </c>
     </row>
@@ -6190,25 +5933,25 @@
         <v>20.7</v>
       </c>
       <c r="F58" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v>14.6349</v>
       </c>
       <c r="G58">
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="H58">
-        <f t="shared" si="17"/>
+        <f>($N$5*G58)*1000</f>
         <v>2.6</v>
       </c>
       <c r="I58">
         <v>1.619</v>
       </c>
       <c r="J58">
-        <f t="shared" si="18"/>
+        <f>(I58/$N$9)*10^6</f>
         <v>161.9</v>
       </c>
       <c r="K58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>323.8</v>
       </c>
     </row>
@@ -6227,25 +5970,25 @@
         <v>13.4</v>
       </c>
       <c r="F59" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v>8.0668000000000006</v>
       </c>
       <c r="G59">
         <v>2.7E-2</v>
       </c>
       <c r="H59">
-        <f t="shared" si="17"/>
+        <f>($N$5*G59)*1000</f>
         <v>1.35</v>
       </c>
       <c r="I59">
         <v>0.877</v>
       </c>
       <c r="J59">
-        <f t="shared" si="18"/>
+        <f>(I59/$N$9)*10^6</f>
         <v>87.7</v>
       </c>
       <c r="K59">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>175.4</v>
       </c>
     </row>
@@ -6307,25 +6050,25 @@
         <v>67.099999999999994</v>
       </c>
       <c r="F62" s="4">
-        <f t="shared" ref="F62:F71" si="20">(D62 * (E62/1000))*1000</f>
+        <f t="shared" ref="F62:F71" si="8">(D62 * (E62/1000))*1000</f>
         <v>101.0526</v>
       </c>
       <c r="G62">
         <v>0.38500000000000001</v>
       </c>
       <c r="H62">
-        <f t="shared" ref="H62:H71" si="21">($P$5*G62)*1000</f>
+        <f>($N$5*G62)*1000</f>
         <v>19.250000000000004</v>
       </c>
       <c r="I62">
         <v>3.1960000000000002</v>
       </c>
       <c r="J62">
-        <f t="shared" ref="J62:J71" si="22">(I62/$P$9)*10^6</f>
+        <f>(I62/$N$9)*10^6</f>
         <v>319.60000000000002</v>
       </c>
       <c r="K62">
-        <f t="shared" ref="K62:K71" si="23">J62*2</f>
+        <f t="shared" ref="K62:K71" si="9">J62*2</f>
         <v>639.20000000000005</v>
       </c>
     </row>
@@ -6344,25 +6087,25 @@
         <v>58.7</v>
       </c>
       <c r="F63" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>82.532200000000003</v>
       </c>
       <c r="G63">
         <v>0.31</v>
       </c>
       <c r="H63">
-        <f t="shared" si="21"/>
+        <f>($N$5*G63)*1000</f>
         <v>15.5</v>
       </c>
       <c r="I63">
         <v>3.19</v>
       </c>
       <c r="J63">
-        <f t="shared" si="22"/>
+        <f>(I63/$N$9)*10^6</f>
         <v>319</v>
       </c>
       <c r="K63">
-        <f t="shared" si="23"/>
+        <f t="shared" si="9"/>
         <v>638</v>
       </c>
     </row>
@@ -6381,25 +6124,25 @@
         <v>48.3</v>
       </c>
       <c r="F64" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>62.983200000000004</v>
       </c>
       <c r="G64">
         <v>0.23400000000000001</v>
       </c>
       <c r="H64">
-        <f t="shared" si="21"/>
+        <f>($N$5*G64)*1000</f>
         <v>11.700000000000003</v>
       </c>
       <c r="I64">
         <v>3.181</v>
       </c>
       <c r="J64">
-        <f t="shared" si="22"/>
+        <f>(I64/$N$9)*10^6</f>
         <v>318.09999999999997</v>
       </c>
       <c r="K64">
-        <f t="shared" si="23"/>
+        <f t="shared" si="9"/>
         <v>636.19999999999993</v>
       </c>
     </row>
@@ -6418,25 +6161,25 @@
         <v>39.799999999999997</v>
       </c>
       <c r="F65" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>47.998799999999996</v>
       </c>
       <c r="G65">
         <v>0.17399999999999999</v>
       </c>
       <c r="H65">
-        <f t="shared" si="21"/>
+        <f>($N$5*G65)*1000</f>
         <v>8.6999999999999993</v>
       </c>
       <c r="I65">
         <v>3.1659999999999999</v>
       </c>
       <c r="J65">
-        <f t="shared" si="22"/>
+        <f>(I65/$N$9)*10^6</f>
         <v>316.60000000000002</v>
       </c>
       <c r="K65">
-        <f t="shared" si="23"/>
+        <f t="shared" si="9"/>
         <v>633.20000000000005</v>
       </c>
     </row>
@@ -6455,25 +6198,25 @@
         <v>35.700000000000003</v>
       </c>
       <c r="F66" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>39.305700000000002</v>
       </c>
       <c r="G66">
         <v>0.14299999999999999</v>
       </c>
       <c r="H66">
-        <f t="shared" si="21"/>
+        <f>($N$5*G66)*1000</f>
         <v>7.15</v>
       </c>
       <c r="I66">
         <v>3.149</v>
       </c>
       <c r="J66">
-        <f t="shared" si="22"/>
+        <f>(I66/$N$9)*10^6</f>
         <v>314.90000000000003</v>
       </c>
       <c r="K66">
-        <f t="shared" si="23"/>
+        <f t="shared" si="9"/>
         <v>629.80000000000007</v>
       </c>
     </row>
@@ -6492,25 +6235,25 @@
         <v>31.8</v>
       </c>
       <c r="F67" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>31.9908</v>
       </c>
       <c r="G67">
         <v>0.115</v>
       </c>
       <c r="H67">
-        <f t="shared" si="21"/>
+        <f>($N$5*G67)*1000</f>
         <v>5.7500000000000009</v>
       </c>
       <c r="I67">
         <v>3.0939999999999999</v>
       </c>
       <c r="J67">
-        <f t="shared" si="22"/>
+        <f>(I67/$N$9)*10^6</f>
         <v>309.39999999999998</v>
       </c>
       <c r="K67">
-        <f t="shared" si="23"/>
+        <f t="shared" si="9"/>
         <v>618.79999999999995</v>
       </c>
     </row>
@@ -6529,25 +6272,25 @@
         <v>27.2</v>
       </c>
       <c r="F68" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>24.697600000000001</v>
       </c>
       <c r="G68">
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="H68">
-        <f t="shared" si="21"/>
+        <f>($N$5*G68)*1000</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="I68">
         <v>2.581</v>
       </c>
       <c r="J68">
-        <f t="shared" si="22"/>
+        <f>(I68/$N$9)*10^6</f>
         <v>258.09999999999997</v>
       </c>
       <c r="K68">
-        <f t="shared" si="23"/>
+        <f t="shared" si="9"/>
         <v>516.19999999999993</v>
       </c>
     </row>
@@ -6566,25 +6309,25 @@
         <v>20.7</v>
       </c>
       <c r="F69" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>16.704900000000002</v>
       </c>
       <c r="G69">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="H69">
-        <f t="shared" si="21"/>
+        <f>($N$5*G69)*1000</f>
         <v>2.85</v>
       </c>
       <c r="I69">
         <v>1.7749999999999999</v>
       </c>
       <c r="J69">
-        <f t="shared" si="22"/>
+        <f>(I69/$N$9)*10^6</f>
         <v>177.49999999999997</v>
       </c>
       <c r="K69">
-        <f t="shared" si="23"/>
+        <f t="shared" si="9"/>
         <v>354.99999999999994</v>
       </c>
     </row>
@@ -6603,25 +6346,25 @@
         <v>14.1</v>
       </c>
       <c r="F70" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>9.9545999999999992</v>
       </c>
       <c r="G70">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="H70">
-        <f t="shared" si="21"/>
+        <f>($N$5*G70)*1000</f>
         <v>1.6</v>
       </c>
       <c r="I70">
         <v>1.0469999999999999</v>
       </c>
       <c r="J70">
-        <f t="shared" si="22"/>
+        <f>(I70/$N$9)*10^6</f>
         <v>104.7</v>
       </c>
       <c r="K70">
-        <f t="shared" si="23"/>
+        <f t="shared" si="9"/>
         <v>209.4</v>
       </c>
     </row>
@@ -6640,25 +6383,25 @@
         <v>7.5</v>
       </c>
       <c r="F71" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>4.5374999999999996</v>
       </c>
       <c r="G71">
         <v>1.2E-2</v>
       </c>
       <c r="H71">
-        <f t="shared" si="21"/>
+        <f>($N$5*G71)*1000</f>
         <v>0.60000000000000009</v>
       </c>
       <c r="I71">
         <v>0.39400000000000002</v>
       </c>
       <c r="J71">
-        <f t="shared" si="22"/>
+        <f>(I71/$N$9)*10^6</f>
         <v>39.400000000000006</v>
       </c>
       <c r="K71">
-        <f t="shared" si="23"/>
+        <f t="shared" si="9"/>
         <v>78.800000000000011</v>
       </c>
     </row>
@@ -6723,25 +6466,25 @@
         <v>60.1</v>
       </c>
       <c r="F74" s="4">
-        <f t="shared" ref="F74:F83" si="24">(D74 * (E74/1000))*1000</f>
+        <f t="shared" ref="F74:F83" si="10">(D74 * (E74/1000))*1000</f>
         <v>90.15</v>
       </c>
       <c r="G74">
         <v>0.34499999999999997</v>
       </c>
       <c r="H74">
-        <f t="shared" ref="H74:H83" si="25">($P$5*G74)*1000</f>
+        <f>($N$5*G74)*1000</f>
         <v>17.249999999999996</v>
       </c>
       <c r="I74">
         <v>3.194</v>
       </c>
       <c r="J74">
-        <f t="shared" ref="J74:J83" si="26">(I74/$P$9)*10^6</f>
+        <f>(I74/$N$9)*10^6</f>
         <v>319.40000000000003</v>
       </c>
       <c r="K74">
-        <f t="shared" ref="K74:K83" si="27">J74*2</f>
+        <f t="shared" ref="K74:K83" si="11">J74*2</f>
         <v>638.80000000000007</v>
       </c>
     </row>
@@ -6760,25 +6503,25 @@
         <v>51.5</v>
       </c>
       <c r="F75" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>72.254499999999993</v>
       </c>
       <c r="G75">
         <v>0.27500000000000002</v>
       </c>
       <c r="H75">
-        <f t="shared" si="25"/>
+        <f>($N$5*G75)*1000</f>
         <v>13.750000000000002</v>
       </c>
       <c r="I75">
         <v>3.1869999999999998</v>
       </c>
       <c r="J75">
-        <f t="shared" si="26"/>
+        <f>(I75/$N$9)*10^6</f>
         <v>318.7</v>
       </c>
       <c r="K75">
-        <f t="shared" si="27"/>
+        <f t="shared" si="11"/>
         <v>637.4</v>
       </c>
     </row>
@@ -6797,25 +6540,25 @@
         <v>42.3</v>
       </c>
       <c r="F76" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>55.032299999999992</v>
       </c>
       <c r="G76">
         <v>0.20499999999999999</v>
       </c>
       <c r="H76">
-        <f t="shared" si="25"/>
+        <f>($N$5*G76)*1000</f>
         <v>10.25</v>
       </c>
       <c r="I76">
         <v>3.1749999999999998</v>
       </c>
       <c r="J76">
-        <f t="shared" si="26"/>
+        <f>(I76/$N$9)*10^6</f>
         <v>317.49999999999994</v>
       </c>
       <c r="K76">
-        <f t="shared" si="27"/>
+        <f t="shared" si="11"/>
         <v>634.99999999999989</v>
       </c>
     </row>
@@ -6834,25 +6577,25 @@
         <v>37.299999999999997</v>
       </c>
       <c r="F77" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>45.095700000000001</v>
       </c>
       <c r="G77">
         <v>0.16600000000000001</v>
       </c>
       <c r="H77">
-        <f t="shared" si="25"/>
+        <f>($N$5*G77)*1000</f>
         <v>8.3000000000000007</v>
       </c>
       <c r="I77">
         <v>3.1629999999999998</v>
       </c>
       <c r="J77">
-        <f t="shared" si="26"/>
+        <f>(I77/$N$9)*10^6</f>
         <v>316.3</v>
       </c>
       <c r="K77">
-        <f t="shared" si="27"/>
+        <f t="shared" si="11"/>
         <v>632.6</v>
       </c>
     </row>
@@ -6871,25 +6614,25 @@
         <v>33.299999999999997</v>
       </c>
       <c r="F78" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>36.796499999999995</v>
       </c>
       <c r="G78">
         <v>0.13400000000000001</v>
       </c>
       <c r="H78">
-        <f t="shared" si="25"/>
+        <f>($N$5*G78)*1000</f>
         <v>6.7000000000000011</v>
       </c>
       <c r="I78">
         <v>3.1419999999999999</v>
       </c>
       <c r="J78">
-        <f t="shared" si="26"/>
+        <f>(I78/$N$9)*10^6</f>
         <v>314.2</v>
       </c>
       <c r="K78">
-        <f t="shared" si="27"/>
+        <f t="shared" si="11"/>
         <v>628.4</v>
       </c>
     </row>
@@ -6908,25 +6651,25 @@
         <v>29.1</v>
       </c>
       <c r="F79" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>29.1873</v>
       </c>
       <c r="G79">
         <v>0.105</v>
       </c>
       <c r="H79">
-        <f t="shared" si="25"/>
+        <f>($N$5*G79)*1000</f>
         <v>5.25</v>
       </c>
       <c r="I79">
         <v>2.964</v>
       </c>
       <c r="J79">
-        <f t="shared" si="26"/>
+        <f>(I79/$N$9)*10^6</f>
         <v>296.39999999999998</v>
       </c>
       <c r="K79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="11"/>
         <v>592.79999999999995</v>
       </c>
     </row>
@@ -6945,25 +6688,25 @@
         <v>23.5</v>
       </c>
       <c r="F80" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>21.196999999999999</v>
       </c>
       <c r="G80">
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="H80">
-        <f t="shared" si="25"/>
+        <f>($N$5*G80)*1000</f>
         <v>3.7</v>
       </c>
       <c r="I80">
         <v>2.2290000000000001</v>
       </c>
       <c r="J80">
-        <f t="shared" si="26"/>
+        <f>(I80/$N$9)*10^6</f>
         <v>222.9</v>
       </c>
       <c r="K80">
-        <f t="shared" si="27"/>
+        <f t="shared" si="11"/>
         <v>445.8</v>
       </c>
     </row>
@@ -6982,25 +6725,25 @@
         <v>17.5</v>
       </c>
       <c r="F81" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>14.105000000000002</v>
       </c>
       <c r="G81">
         <v>4.7E-2</v>
       </c>
       <c r="H81">
-        <f t="shared" si="25"/>
+        <f>($N$5*G81)*1000</f>
         <v>2.35</v>
       </c>
       <c r="I81">
         <v>1.49</v>
       </c>
       <c r="J81">
-        <f t="shared" si="26"/>
+        <f>(I81/$N$9)*10^6</f>
         <v>149</v>
       </c>
       <c r="K81">
-        <f t="shared" si="27"/>
+        <f t="shared" si="11"/>
         <v>298</v>
       </c>
     </row>
@@ -7019,25 +6762,25 @@
         <v>12</v>
       </c>
       <c r="F82" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>8.4479999999999986</v>
       </c>
       <c r="G82">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="H82">
-        <f t="shared" si="25"/>
+        <f>($N$5*G82)*1000</f>
         <v>1.3</v>
       </c>
       <c r="I82">
         <v>0.86099999999999999</v>
       </c>
       <c r="J82">
-        <f t="shared" si="26"/>
+        <f>(I82/$N$9)*10^6</f>
         <v>86.1</v>
       </c>
       <c r="K82">
-        <f t="shared" si="27"/>
+        <f t="shared" si="11"/>
         <v>172.2</v>
       </c>
     </row>
@@ -7056,25 +6799,25 @@
         <v>5.3</v>
       </c>
       <c r="F83" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>3.1905999999999999</v>
       </c>
       <c r="G83">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="H83">
-        <f t="shared" si="25"/>
+        <f>($N$5*G83)*1000</f>
         <v>0.35000000000000003</v>
       </c>
       <c r="I83">
         <v>0.221</v>
       </c>
       <c r="J83">
-        <f t="shared" si="26"/>
+        <f>(I83/$N$9)*10^6</f>
         <v>22.1</v>
       </c>
       <c r="K83">
-        <f t="shared" si="27"/>
+        <f t="shared" si="11"/>
         <v>44.2</v>
       </c>
     </row>
@@ -7136,25 +6879,25 @@
         <v>52.6</v>
       </c>
       <c r="F86" s="4">
-        <f t="shared" ref="F86:F95" si="28">(D86 * (E86/1000))*1000</f>
+        <f t="shared" ref="F86:F95" si="12">(D86 * (E86/1000))*1000</f>
         <v>79.0578</v>
       </c>
       <c r="G86">
         <v>0.307</v>
       </c>
       <c r="H86">
-        <f t="shared" ref="H86:H95" si="29">($P$5*G86)*1000</f>
+        <f>($N$5*G86)*1000</f>
         <v>15.350000000000001</v>
       </c>
       <c r="I86">
         <v>3.1930000000000001</v>
       </c>
       <c r="J86">
-        <f t="shared" ref="J86:J95" si="30">(I86/$P$9)*10^6</f>
+        <f>(I86/$N$9)*10^6</f>
         <v>319.3</v>
       </c>
       <c r="K86">
-        <f t="shared" ref="K86:K95" si="31">J86*2</f>
+        <f t="shared" ref="K86:K95" si="13">J86*2</f>
         <v>638.6</v>
       </c>
     </row>
@@ -7173,25 +6916,25 @@
         <v>44.1</v>
       </c>
       <c r="F87" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="12"/>
         <v>61.828200000000002</v>
       </c>
       <c r="G87">
         <v>0.23699999999999999</v>
       </c>
       <c r="H87">
-        <f t="shared" si="29"/>
+        <f>($N$5*G87)*1000</f>
         <v>11.85</v>
       </c>
       <c r="I87">
         <v>3.1829999999999998</v>
       </c>
       <c r="J87">
-        <f t="shared" si="30"/>
+        <f>(I87/$N$9)*10^6</f>
         <v>318.3</v>
       </c>
       <c r="K87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="13"/>
         <v>636.6</v>
       </c>
     </row>
@@ -7210,25 +6953,25 @@
         <v>37.6</v>
       </c>
       <c r="F88" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="12"/>
         <v>49.180800000000005</v>
       </c>
       <c r="G88">
         <v>0.185</v>
       </c>
       <c r="H88">
-        <f t="shared" si="29"/>
+        <f>($N$5*G88)*1000</f>
         <v>9.25</v>
       </c>
       <c r="I88">
         <v>3.1709999999999998</v>
       </c>
       <c r="J88">
-        <f t="shared" si="30"/>
+        <f>(I88/$N$9)*10^6</f>
         <v>317.09999999999997</v>
       </c>
       <c r="K88">
-        <f t="shared" si="31"/>
+        <f t="shared" si="13"/>
         <v>634.19999999999993</v>
       </c>
     </row>
@@ -7247,25 +6990,25 @@
         <v>33.700000000000003</v>
       </c>
       <c r="F89" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="12"/>
         <v>40.5411</v>
       </c>
       <c r="G89">
         <v>0.15</v>
       </c>
       <c r="H89">
-        <f t="shared" si="29"/>
+        <f>($N$5*G89)*1000</f>
         <v>7.5</v>
       </c>
       <c r="I89">
         <v>3.157</v>
       </c>
       <c r="J89">
-        <f t="shared" si="30"/>
+        <f>(I89/$N$9)*10^6</f>
         <v>315.7</v>
       </c>
       <c r="K89">
-        <f t="shared" si="31"/>
+        <f t="shared" si="13"/>
         <v>631.4</v>
       </c>
     </row>
@@ -7284,25 +7027,25 @@
         <v>30.1</v>
       </c>
       <c r="F90" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="12"/>
         <v>33.320700000000002</v>
       </c>
       <c r="G90">
         <v>0.121</v>
       </c>
       <c r="H90">
-        <f t="shared" si="29"/>
+        <f>($N$5*G90)*1000</f>
         <v>6.05</v>
       </c>
       <c r="I90">
         <v>3.1240000000000001</v>
       </c>
       <c r="J90">
-        <f t="shared" si="30"/>
+        <f>(I90/$N$9)*10^6</f>
         <v>312.39999999999998</v>
       </c>
       <c r="K90">
-        <f t="shared" si="31"/>
+        <f t="shared" si="13"/>
         <v>624.79999999999995</v>
       </c>
     </row>
@@ -7321,25 +7064,25 @@
         <v>25.45</v>
       </c>
       <c r="F91" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="12"/>
         <v>25.653600000000001</v>
       </c>
       <c r="G91">
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="H91">
-        <f t="shared" si="29"/>
+        <f>($N$5*G91)*1000</f>
         <v>4.55</v>
       </c>
       <c r="I91">
         <v>2.66</v>
       </c>
       <c r="J91">
-        <f t="shared" si="30"/>
+        <f>(I91/$N$9)*10^6</f>
         <v>266</v>
       </c>
       <c r="K91">
-        <f t="shared" si="31"/>
+        <f t="shared" si="13"/>
         <v>532</v>
       </c>
     </row>
@@ -7358,25 +7101,25 @@
         <v>19.7</v>
       </c>
       <c r="F92" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="12"/>
         <v>17.887599999999999</v>
       </c>
       <c r="G92">
         <v>0.06</v>
       </c>
       <c r="H92">
-        <f t="shared" si="29"/>
+        <f>($N$5*G92)*1000</f>
         <v>3</v>
       </c>
       <c r="I92">
         <v>1.877</v>
       </c>
       <c r="J92">
-        <f t="shared" si="30"/>
+        <f>(I92/$N$9)*10^6</f>
         <v>187.70000000000002</v>
       </c>
       <c r="K92">
-        <f t="shared" si="31"/>
+        <f t="shared" si="13"/>
         <v>375.40000000000003</v>
       </c>
     </row>
@@ -7395,25 +7138,25 @@
         <v>15.1</v>
       </c>
       <c r="F93" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="12"/>
         <v>12.2159</v>
       </c>
       <c r="G93">
         <v>3.9E-2</v>
       </c>
       <c r="H93">
-        <f t="shared" si="29"/>
+        <f>($N$5*G93)*1000</f>
         <v>1.9500000000000002</v>
       </c>
       <c r="I93">
         <v>1.2649999999999999</v>
       </c>
       <c r="J93">
-        <f t="shared" si="30"/>
+        <f>(I93/$N$9)*10^6</f>
         <v>126.49999999999999</v>
       </c>
       <c r="K93">
-        <f t="shared" si="31"/>
+        <f t="shared" si="13"/>
         <v>252.99999999999997</v>
       </c>
     </row>
@@ -7432,25 +7175,25 @@
         <v>9.6</v>
       </c>
       <c r="F94" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="12"/>
         <v>6.7679999999999989</v>
       </c>
       <c r="G94">
         <v>1.9E-2</v>
       </c>
       <c r="H94">
-        <f t="shared" si="29"/>
+        <f>($N$5*G94)*1000</f>
         <v>0.95</v>
       </c>
       <c r="I94">
         <v>0.629</v>
       </c>
       <c r="J94">
-        <f t="shared" si="30"/>
+        <f>(I94/$N$9)*10^6</f>
         <v>62.9</v>
       </c>
       <c r="K94">
-        <f t="shared" si="31"/>
+        <f t="shared" si="13"/>
         <v>125.8</v>
       </c>
     </row>
@@ -7469,25 +7212,25 @@
         <v>3.7</v>
       </c>
       <c r="F95" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="12"/>
         <v>2.2458999999999998</v>
       </c>
       <c r="G95">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="H95">
-        <f t="shared" si="29"/>
+        <f>($N$5*G95)*1000</f>
         <v>0.2</v>
       </c>
       <c r="I95">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="J95">
-        <f t="shared" si="30"/>
+        <f>(I95/$N$9)*10^6</f>
         <v>8.4</v>
       </c>
       <c r="K95">
-        <f t="shared" si="31"/>
+        <f t="shared" si="13"/>
         <v>16.8</v>
       </c>
     </row>
@@ -7512,8 +7255,8 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
   <tableParts count="8">
+    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
@@ -7521,7 +7264,6 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
-    <tablePart r:id="rId10"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>